<commit_message>
- AlpsNMR.Rproj removed from git repository - Reduced demo dataset to avoid package size > 5 MB - Modified introduction to alpsnmr vignette and some tests   to work with reduced demo dataset
</commit_message>
<xml_diff>
--- a/inst/dataset-demo/dummy_metadata.xlsx
+++ b/inst/dataset-demo/dummy_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmadrid\Documents\IBEC\NESTLE\code\AlpsNMR-master\inst\dataset-demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hgracia\Desktop\IBEC\AlpsNMR\inst\dataset-demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB60DC5A-2C6C-4CF3-AC0A-11C65ECE1E94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17185FC9-EAFC-4279-9A0A-93FFE27B8419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>NMRExperiment</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Elia</t>
-  </si>
-  <si>
-    <t>40</t>
   </si>
   <si>
     <t>Age</t>
@@ -443,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,10 +456,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -470,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -481,10 +478,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -492,17 +489,6 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -517,17 +503,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -535,7 +521,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>

</xml_diff>